<commit_message>
Added helical new measurements and full data
</commit_message>
<xml_diff>
--- a/FullData2.xlsx
+++ b/FullData2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian\Programming\bluetoothping\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Degrees</t>
   </si>
@@ -106,6 +106,12 @@
   <si>
     <t>Helical Signal Strength</t>
   </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             </t>
+  </si>
 </sst>
 </file>
 
@@ -115,7 +121,7 @@
     <numFmt numFmtId="164" formatCode="###\°"/>
     <numFmt numFmtId="165" formatCode="####\°"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,16 +129,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -140,17 +446,208 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -245,7 +742,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$25</c:f>
               <c:numCache>
-                <c:formatCode>###\°</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -347,7 +844,7 @@
                   <c:v>-20.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-10.666666666666666</c:v>
+                  <c:v>-12.333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-12.666666666666666</c:v>
@@ -398,7 +895,7 @@
                   <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-14.333333333333334</c:v>
+                  <c:v>-14.666666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -464,7 +961,7 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>###\°</c:formatCode>
+                      <c:formatCode>General</c:formatCode>
                       <c:ptCount val="24"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
@@ -551,7 +1048,7 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>###\°</c:formatCode>
+                      <c:formatCode>General</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
@@ -624,7 +1121,7 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>###\°</c:formatCode>
+                      <c:formatCode>General</c:formatCode>
                       <c:ptCount val="24"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
@@ -784,7 +1281,7 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>###\°</c:formatCode>
+                      <c:formatCode>General</c:formatCode>
                       <c:ptCount val="24"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
@@ -944,7 +1441,7 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>###\°</c:formatCode>
+                      <c:formatCode>General</c:formatCode>
                       <c:ptCount val="24"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
@@ -1071,7 +1568,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="###\°" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3918,7 +4415,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$80:$A$103</c15:sqref>
@@ -4078,7 +4575,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$80:$A$103</c15:sqref>
@@ -4238,7 +4735,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$80:$A$103</c15:sqref>
@@ -4745,76 +5242,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>-29.666666666666668</c:v>
+                  <c:v>-11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-22.333333333333332</c:v>
+                  <c:v>-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-25.666666666666668</c:v>
+                  <c:v>-13.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-24</c:v>
+                  <c:v>-17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-18.666666666666668</c:v>
+                  <c:v>-14.333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-19.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>-21.666666666666668</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="12">
+                  <c:v>-21.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-15.333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>-14.666666666666666</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="15">
+                  <c:v>-17.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-18.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-14.666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>-12.666666666666666</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-10.333333333333334</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-11.333333333333334</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-16.666666666666668</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-15.333333333333334</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-21.666666666666668</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-21.333333333333332</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-23</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-16.666666666666668</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-18</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-21.666666666666668</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-24.333333333333332</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8395,15 +8892,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>22416</xdr:colOff>
+      <xdr:colOff>22415</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>44821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>446959</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>44821</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>251015</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>82921</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8436,10 +8933,10 @@
       <xdr:rowOff>27970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>267661</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>27970</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>112539</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>66070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8467,15 +8964,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>28158</xdr:colOff>
+      <xdr:colOff>28157</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>37547</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>452701</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>37547</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>256757</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>75647</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8508,10 +9005,10 @@
       <xdr:rowOff>40893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>257973</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>40893</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>102851</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>78993</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8539,15 +9036,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>13608</xdr:colOff>
+      <xdr:colOff>13607</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>13608</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>438151</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>13608</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>242207</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>51708</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8874,10 +9371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ131"/>
+  <dimension ref="A1:AU131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8900,16 +9397,16 @@
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>-22</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>-25</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>-24</v>
       </c>
       <c r="E2">
@@ -8918,16 +9415,16 @@
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>15</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>-16</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>-18</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>-16</v>
       </c>
       <c r="E3">
@@ -8936,16 +9433,16 @@
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>30</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>-18</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>-18</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>-18</v>
       </c>
       <c r="E4">
@@ -8954,16 +9451,16 @@
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <v>45</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>-15</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>-15</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>-18</v>
       </c>
       <c r="E5">
@@ -8972,16 +9469,16 @@
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="4">
         <v>60</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>-22</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>-23</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>-21</v>
       </c>
       <c r="E6">
@@ -8996,16 +9493,16 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="4">
         <v>75</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>-25</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>-21</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>-15</v>
       </c>
       <c r="E7">
@@ -9014,34 +9511,34 @@
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="4">
         <v>90</v>
       </c>
-      <c r="B8">
-        <v>-11</v>
-      </c>
-      <c r="C8">
-        <v>-11</v>
-      </c>
-      <c r="D8">
+      <c r="B8" s="4">
+        <v>-12</v>
+      </c>
+      <c r="C8" s="4">
+        <v>-15</v>
+      </c>
+      <c r="D8" s="4">
         <v>-10</v>
       </c>
       <c r="E8">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-10.666666666666666</v>
+        <v>-12.333333333333334</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="4">
         <v>105</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>-13</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>-12</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>-13</v>
       </c>
       <c r="E9">
@@ -9053,16 +9550,16 @@
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="4">
         <v>120</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>-18</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>-19</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>-18</v>
       </c>
       <c r="E10">
@@ -9071,16 +9568,16 @@
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="4">
         <v>135</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>-17</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>-17</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>-18</v>
       </c>
       <c r="E11">
@@ -9092,16 +9589,16 @@
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="4">
         <v>150</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>-18</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>-18</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>-18</v>
       </c>
       <c r="E12">
@@ -9110,16 +9607,16 @@
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="4">
         <v>165</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>-15</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>-19</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>-19</v>
       </c>
       <c r="E13">
@@ -9128,16 +9625,16 @@
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="4">
         <v>180</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>-18</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>-16</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>-16</v>
       </c>
       <c r="E14">
@@ -9146,16 +9643,16 @@
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="4">
         <v>195</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4">
         <v>-14</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>-14</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>-14</v>
       </c>
       <c r="E15">
@@ -9164,16 +9661,16 @@
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="4">
         <v>210</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>-15</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>-13</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>-15</v>
       </c>
       <c r="E16">
@@ -9182,16 +9679,16 @@
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="4">
         <v>225</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>-12</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>-12</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>-12</v>
       </c>
       <c r="E17">
@@ -9203,16 +9700,16 @@
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="4">
         <v>240</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>-10</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>-10</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>-8</v>
       </c>
       <c r="E18">
@@ -9221,16 +9718,16 @@
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="4">
         <v>255</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>-16</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>-15</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>-16</v>
       </c>
       <c r="E19">
@@ -9239,16 +9736,16 @@
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="4">
         <v>270</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4">
         <v>-13</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>-12</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>-12</v>
       </c>
       <c r="E20">
@@ -9257,16 +9754,16 @@
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="4">
         <v>285</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>-12</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>-11</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>-11</v>
       </c>
       <c r="E21">
@@ -9275,16 +9772,16 @@
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="4">
         <v>300</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <v>-15</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>-13</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>-15</v>
       </c>
       <c r="E22">
@@ -9293,16 +9790,16 @@
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="4">
         <v>315</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>-23</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>-23</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>-22</v>
       </c>
       <c r="E23">
@@ -9311,16 +9808,16 @@
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="4">
         <v>330</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4">
         <v>-16</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>-16</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <v>-16</v>
       </c>
       <c r="E24">
@@ -9329,27 +9826,27 @@
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="4">
         <v>345</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4">
         <v>-14</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <v>-15</v>
       </c>
-      <c r="D25">
-        <v>-14</v>
+      <c r="D25" s="4">
+        <v>-15</v>
       </c>
       <c r="E25">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-14.333333333333334</v>
+        <v>-14.666666666666666</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="E26">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())):(INDIRECT(ADDRESS(ROW()-24,COLUMN()))))</f>
-        <v>-16.013888888888886</v>
+        <v>-16.097222222222221</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
@@ -10040,7 +10537,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>165</v>
       </c>
@@ -10058,7 +10555,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>180</v>
       </c>
@@ -10076,7 +10573,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>195</v>
       </c>
@@ -10094,7 +10591,7 @@
         <v>-20.333333333333332</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>210</v>
       </c>
@@ -10112,7 +10609,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>225</v>
       </c>
@@ -10130,7 +10627,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>240</v>
       </c>
@@ -10147,8 +10644,11 @@
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
         <v>-9</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="AU70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>255</v>
       </c>
@@ -10166,7 +10666,7 @@
         <v>-8.6666666666666661</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>270</v>
       </c>
@@ -10184,7 +10684,7 @@
         <v>-5.666666666666667</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>285</v>
       </c>
@@ -10202,7 +10702,7 @@
         <v>-6.333333333333333</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>300</v>
       </c>
@@ -10220,7 +10720,7 @@
         <v>-6.333333333333333</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>315</v>
       </c>
@@ -10238,7 +10738,7 @@
         <v>-10.666666666666666</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>330</v>
       </c>
@@ -10256,7 +10756,7 @@
         <v>-18.666666666666668</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>345</v>
       </c>
@@ -10274,13 +10774,12 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E78">
-        <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())):(INDIRECT(ADDRESS(ROW()-24,COLUMN()))))</f>
-        <v>-13.291666666666666</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -10297,7 +10796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>0</v>
       </c>
@@ -10756,444 +11255,444 @@
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A107">
+      <c r="A107" s="3">
         <v>0</v>
       </c>
-      <c r="B107">
-        <v>-30</v>
-      </c>
-      <c r="C107">
-        <v>-30</v>
-      </c>
-      <c r="D107">
-        <v>-29</v>
+      <c r="B107" s="3">
+        <v>-11</v>
+      </c>
+      <c r="C107" s="3">
+        <v>-11</v>
+      </c>
+      <c r="D107" s="3">
+        <v>-11</v>
       </c>
       <c r="E107">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-29.666666666666668</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A108">
+      <c r="A108" s="3">
         <v>15</v>
       </c>
-      <c r="B108">
-        <v>-23</v>
-      </c>
-      <c r="C108">
-        <v>-22</v>
-      </c>
-      <c r="D108">
-        <v>-22</v>
+      <c r="B108" s="3">
+        <v>-8</v>
+      </c>
+      <c r="C108" s="3">
+        <v>-8</v>
+      </c>
+      <c r="D108" s="3">
+        <v>-8</v>
       </c>
       <c r="E108">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-22.333333333333332</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A109">
+      <c r="A109" s="3">
         <v>30</v>
       </c>
-      <c r="B109">
-        <v>-26</v>
-      </c>
-      <c r="C109">
-        <v>-26</v>
-      </c>
-      <c r="D109">
-        <v>-25</v>
+      <c r="B109" s="3">
+        <v>-14</v>
+      </c>
+      <c r="C109" s="3">
+        <v>-14</v>
+      </c>
+      <c r="D109" s="3">
+        <v>-13</v>
       </c>
       <c r="E109">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-25.666666666666668</v>
+        <v>-13.666666666666666</v>
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A110">
+      <c r="A110" s="3">
         <v>45</v>
       </c>
-      <c r="B110">
-        <v>-24</v>
-      </c>
-      <c r="C110">
-        <v>-24</v>
-      </c>
-      <c r="D110">
-        <v>-24</v>
+      <c r="B110" s="3">
+        <v>-17</v>
+      </c>
+      <c r="C110" s="3">
+        <v>-17</v>
+      </c>
+      <c r="D110" s="3">
+        <v>-17</v>
       </c>
       <c r="E110">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-24</v>
+        <v>-17</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A111">
+      <c r="A111" s="3">
         <v>60</v>
       </c>
-      <c r="B111">
-        <v>-17</v>
-      </c>
-      <c r="C111">
+      <c r="B111" s="3">
+        <v>-15</v>
+      </c>
+      <c r="C111" s="3">
+        <v>-14</v>
+      </c>
+      <c r="D111" s="3">
+        <v>-14</v>
+      </c>
+      <c r="E111">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-14.333333333333334</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
+        <v>75</v>
+      </c>
+      <c r="B112" s="3">
+        <v>-21</v>
+      </c>
+      <c r="C112" s="3">
+        <v>-21</v>
+      </c>
+      <c r="D112" s="3">
+        <v>-21</v>
+      </c>
+      <c r="E112">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
+        <v>90</v>
+      </c>
+      <c r="B113" s="3">
         <v>-20</v>
       </c>
-      <c r="D111">
+      <c r="C113" s="3">
         <v>-19</v>
       </c>
-      <c r="E111">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-18.666666666666668</v>
-      </c>
-    </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>75</v>
-      </c>
-      <c r="B112">
-        <v>-23</v>
-      </c>
-      <c r="C112">
+      <c r="D113" s="3">
+        <v>-19</v>
+      </c>
+      <c r="E113">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-19.333333333333332</v>
+      </c>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
+        <v>105</v>
+      </c>
+      <c r="B114" s="3">
+        <v>-18</v>
+      </c>
+      <c r="C114" s="3">
+        <v>-18</v>
+      </c>
+      <c r="D114" s="3">
+        <v>-18</v>
+      </c>
+      <c r="E114">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A115" s="3">
+        <v>120</v>
+      </c>
+      <c r="B115" s="3">
+        <v>-14</v>
+      </c>
+      <c r="C115" s="3">
+        <v>-14</v>
+      </c>
+      <c r="D115" s="3">
+        <v>-14</v>
+      </c>
+      <c r="E115">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
+        <v>135</v>
+      </c>
+      <c r="B116" s="3">
         <v>-20</v>
       </c>
-      <c r="D112">
-        <v>-22</v>
-      </c>
-      <c r="E112">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-21.666666666666668</v>
-      </c>
-    </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A113">
-        <v>90</v>
-      </c>
-      <c r="B113">
-        <v>-18</v>
-      </c>
-      <c r="C113">
-        <v>-15</v>
-      </c>
-      <c r="D113">
-        <v>-11</v>
-      </c>
-      <c r="E113">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-14.666666666666666</v>
-      </c>
-    </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>105</v>
-      </c>
-      <c r="B114">
-        <v>-13</v>
-      </c>
-      <c r="C114">
-        <v>-14</v>
-      </c>
-      <c r="D114">
-        <v>-11</v>
-      </c>
-      <c r="E114">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-12.666666666666666</v>
-      </c>
-    </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>120</v>
-      </c>
-      <c r="B115">
-        <v>-10</v>
-      </c>
-      <c r="C115">
-        <v>-10</v>
-      </c>
-      <c r="D115">
-        <v>-11</v>
-      </c>
-      <c r="E115">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-10.333333333333334</v>
-      </c>
-    </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>135</v>
-      </c>
-      <c r="B116">
-        <v>-8</v>
-      </c>
-      <c r="C116">
-        <v>-8</v>
-      </c>
-      <c r="D116">
-        <v>-8</v>
+      <c r="C116" s="3">
+        <v>-20</v>
+      </c>
+      <c r="D116" s="3">
+        <v>-20</v>
       </c>
       <c r="E116">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-8</v>
+        <v>-20</v>
       </c>
       <c r="U116" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A117">
+      <c r="A117" s="3">
         <v>150</v>
       </c>
-      <c r="B117">
-        <v>-7</v>
-      </c>
-      <c r="C117">
-        <v>-6</v>
-      </c>
-      <c r="D117">
-        <v>-5</v>
+      <c r="B117" s="3">
+        <v>-21</v>
+      </c>
+      <c r="C117" s="3">
+        <v>-21</v>
+      </c>
+      <c r="D117" s="3">
+        <v>-21</v>
       </c>
       <c r="E117">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-6</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118">
+      <c r="A118" s="3">
         <v>165</v>
       </c>
-      <c r="B118">
-        <v>-12</v>
-      </c>
-      <c r="C118">
+      <c r="B118" s="3">
+        <v>-22</v>
+      </c>
+      <c r="C118" s="3">
+        <v>-21</v>
+      </c>
+      <c r="D118" s="3">
+        <v>-22</v>
+      </c>
+      <c r="E118">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-21.666666666666668</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
+        <v>180</v>
+      </c>
+      <c r="B119" s="3">
+        <v>-22</v>
+      </c>
+      <c r="C119" s="3">
+        <v>-20</v>
+      </c>
+      <c r="D119" s="3">
+        <v>-22</v>
+      </c>
+      <c r="E119">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-21.333333333333332</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A120" s="3">
+        <v>195</v>
+      </c>
+      <c r="B120" s="3">
+        <v>-16</v>
+      </c>
+      <c r="C120" s="3">
         <v>-14</v>
       </c>
-      <c r="D118">
+      <c r="D120" s="3">
+        <v>-16</v>
+      </c>
+      <c r="E120">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-15.333333333333334</v>
+      </c>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A121" s="3">
+        <v>210</v>
+      </c>
+      <c r="B121" s="3">
+        <v>-15</v>
+      </c>
+      <c r="C121" s="3">
+        <v>-15</v>
+      </c>
+      <c r="D121" s="3">
+        <v>-14</v>
+      </c>
+      <c r="E121">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-14.666666666666666</v>
+      </c>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A122" s="3">
+        <v>225</v>
+      </c>
+      <c r="B122" s="3">
+        <v>-17</v>
+      </c>
+      <c r="C122" s="3">
+        <v>-17</v>
+      </c>
+      <c r="D122" s="3">
+        <v>-18</v>
+      </c>
+      <c r="E122">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-17.333333333333332</v>
+      </c>
+    </row>
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A123" s="3">
+        <v>240</v>
+      </c>
+      <c r="B123" s="3">
+        <v>-19</v>
+      </c>
+      <c r="C123" s="3">
+        <v>-18</v>
+      </c>
+      <c r="D123" s="3">
+        <v>-18</v>
+      </c>
+      <c r="E123">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-18.333333333333332</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A124" s="3">
+        <v>255</v>
+      </c>
+      <c r="B124" s="3">
+        <v>-20</v>
+      </c>
+      <c r="C124" s="3">
+        <v>-20</v>
+      </c>
+      <c r="D124" s="3">
+        <v>-20</v>
+      </c>
+      <c r="E124">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A125" s="3">
+        <v>270</v>
+      </c>
+      <c r="B125" s="3">
+        <v>-15</v>
+      </c>
+      <c r="C125" s="3">
+        <v>-15</v>
+      </c>
+      <c r="D125" s="3">
+        <v>-15</v>
+      </c>
+      <c r="E125">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A126" s="3">
+        <v>285</v>
+      </c>
+      <c r="B126" s="3">
+        <v>-15</v>
+      </c>
+      <c r="C126" s="3">
+        <v>-15</v>
+      </c>
+      <c r="D126" s="3">
+        <v>-15</v>
+      </c>
+      <c r="E126">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A127" s="3">
+        <v>300</v>
+      </c>
+      <c r="B127" s="3">
+        <v>-14</v>
+      </c>
+      <c r="C127" s="3">
+        <v>-14</v>
+      </c>
+      <c r="D127" s="3">
+        <v>-14</v>
+      </c>
+      <c r="E127">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A128" s="3">
+        <v>315</v>
+      </c>
+      <c r="B128" s="3">
+        <v>-14</v>
+      </c>
+      <c r="C128" s="3">
+        <v>-14</v>
+      </c>
+      <c r="D128" s="3">
+        <v>-14</v>
+      </c>
+      <c r="E128">
+        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="3">
+        <v>330</v>
+      </c>
+      <c r="B129" s="4">
+        <v>-15</v>
+      </c>
+      <c r="C129" s="3">
+        <v>-16</v>
+      </c>
+      <c r="D129" s="3">
         <v>-13</v>
       </c>
-      <c r="E118">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A119">
-        <v>180</v>
-      </c>
-      <c r="B119">
-        <v>-11</v>
-      </c>
-      <c r="C119">
-        <v>-11</v>
-      </c>
-      <c r="D119">
-        <v>-12</v>
-      </c>
-      <c r="E119">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-11.333333333333334</v>
-      </c>
-    </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A120">
-        <v>195</v>
-      </c>
-      <c r="B120">
-        <v>-16</v>
-      </c>
-      <c r="C120">
-        <v>-17</v>
-      </c>
-      <c r="D120">
-        <v>-17</v>
-      </c>
-      <c r="E120">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-16.666666666666668</v>
-      </c>
-    </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>210</v>
-      </c>
-      <c r="B121">
-        <v>-15</v>
-      </c>
-      <c r="C121">
-        <v>-15</v>
-      </c>
-      <c r="D121">
-        <v>-16</v>
-      </c>
-      <c r="E121">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-15.333333333333334</v>
-      </c>
-    </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>225</v>
-      </c>
-      <c r="B122">
-        <v>-23</v>
-      </c>
-      <c r="C122">
-        <v>-22</v>
-      </c>
-      <c r="D122">
-        <v>-20</v>
-      </c>
-      <c r="E122">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-21.666666666666668</v>
-      </c>
-    </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A123">
-        <v>240</v>
-      </c>
-      <c r="B123">
-        <v>-21</v>
-      </c>
-      <c r="C123">
-        <v>-21</v>
-      </c>
-      <c r="D123">
-        <v>-22</v>
-      </c>
-      <c r="E123">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-21.333333333333332</v>
-      </c>
-    </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A124">
-        <v>255</v>
-      </c>
-      <c r="B124">
-        <v>-22</v>
-      </c>
-      <c r="C124">
-        <v>-23</v>
-      </c>
-      <c r="D124">
-        <v>-24</v>
-      </c>
-      <c r="E124">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-23</v>
-      </c>
-    </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>270</v>
-      </c>
-      <c r="B125">
-        <v>-11</v>
-      </c>
-      <c r="C125">
-        <v>-11</v>
-      </c>
-      <c r="D125">
-        <v>-11</v>
-      </c>
-      <c r="E125">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-11</v>
-      </c>
-    </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <v>285</v>
-      </c>
-      <c r="B126">
-        <v>-17</v>
-      </c>
-      <c r="C126">
-        <v>-17</v>
-      </c>
-      <c r="D126">
-        <v>-16</v>
-      </c>
-      <c r="E126">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-16.666666666666668</v>
-      </c>
-    </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A127">
-        <v>300</v>
-      </c>
-      <c r="B127">
-        <v>-18</v>
-      </c>
-      <c r="C127">
-        <v>-18</v>
-      </c>
-      <c r="D127">
-        <v>-18</v>
-      </c>
-      <c r="E127">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A128">
-        <v>315</v>
-      </c>
-      <c r="B128">
-        <v>-20</v>
-      </c>
-      <c r="C128">
-        <v>-23</v>
-      </c>
-      <c r="D128">
-        <v>-22</v>
-      </c>
-      <c r="E128">
-        <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-21.666666666666668</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129">
-        <v>330</v>
-      </c>
-      <c r="B129">
-        <v>-21</v>
-      </c>
-      <c r="C129">
-        <v>-26</v>
-      </c>
-      <c r="D129">
-        <v>-26</v>
-      </c>
       <c r="E129">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-24.333333333333332</v>
+        <v>-14.666666666666666</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130">
+      <c r="A130" s="3">
         <v>345</v>
       </c>
-      <c r="B130">
-        <v>-18</v>
-      </c>
-      <c r="C130">
-        <v>-18</v>
-      </c>
-      <c r="D130">
-        <v>-18</v>
+      <c r="B130" s="4">
+        <v>-19</v>
+      </c>
+      <c r="C130" s="3">
+        <v>-10</v>
+      </c>
+      <c r="D130" s="3">
+        <v>-9</v>
       </c>
       <c r="E130">
         <f ca="1">AVERAGE(INDIRECT("RC[-3]",0):INDIRECT("RC[-1]",0))</f>
-        <v>-18</v>
+        <v>-12.666666666666666</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E131">
         <f ca="1">AVERAGE(INDIRECT(ADDRESS(ROW()-1,COLUMN())):(INDIRECT(ADDRESS(ROW()-24,COLUMN()))))</f>
-        <v>-17.736111111111111</v>
+        <v>-16.305555555555554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>